<commit_message>
assign region based on country mapping
</commit_message>
<xml_diff>
--- a/Revenue_Target.xlsx
+++ b/Revenue_Target.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\midhu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Customer_Segmentation_CLV_Engine_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B1A3DE-91DE-429D-9CA8-D2FEEA86ECB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE58A6DC-5E4E-4BEE-9550-DAE022E13CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="revenue_target" sheetId="1" r:id="rId1"/>
@@ -126,11 +126,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,7 +439,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,8 +471,8 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2">
-        <v>150000</v>
+      <c r="D2" s="2">
+        <v>45000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -484,8 +485,8 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3">
-        <v>180000</v>
+      <c r="D3" s="2">
+        <v>130000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -498,8 +499,8 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D4">
-        <v>175000</v>
+      <c r="D4" s="2">
+        <v>45000</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -512,8 +513,8 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5">
-        <v>200000</v>
+      <c r="D5" s="2">
+        <v>85000</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -526,8 +527,8 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6">
-        <v>210000</v>
+      <c r="D6" s="2">
+        <v>95000</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -540,8 +541,8 @@
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7">
-        <v>220000</v>
+      <c r="D7" s="2">
+        <v>100000</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -554,8 +555,8 @@
       <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="D8">
-        <v>230000</v>
+      <c r="D8" s="2">
+        <v>125000</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -568,8 +569,8 @@
       <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D9">
-        <v>225000</v>
+      <c r="D9" s="2">
+        <v>130000</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -582,8 +583,8 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="D10">
-        <v>240000</v>
+      <c r="D10" s="2">
+        <v>190000</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -596,8 +597,8 @@
       <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="D11">
-        <v>250000</v>
+      <c r="D11" s="2">
+        <v>450000</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -610,8 +611,8 @@
       <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="D12">
-        <v>260000</v>
+      <c r="D12" s="2">
+        <v>700000</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -624,8 +625,8 @@
       <c r="C13" t="s">
         <v>15</v>
       </c>
-      <c r="D13">
-        <v>270000</v>
+      <c r="D13" s="2">
+        <v>300000</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -638,8 +639,8 @@
       <c r="C14" t="s">
         <v>4</v>
       </c>
-      <c r="D14">
-        <v>280000</v>
+      <c r="D14" s="2">
+        <v>350000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>